<commit_message>
arrego de errores en los test de postman / agregado test de ejecucion y lista de defectos
</commit_message>
<xml_diff>
--- a/Testing/Template Casos de Prueba - Grupo 1.xlsx
+++ b/Testing/Template Casos de Prueba - Grupo 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Proyecto final\grupo-01\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8022979-BFEE-45AA-87E7-E727623CE9D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF2F268-65CC-49C5-BEFB-41A4A81871FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4065" yWindow="4005" windowWidth="21600" windowHeight="11445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="92">
   <si>
     <t>Id</t>
   </si>
@@ -258,6 +258,45 @@
   <si>
     <t>La pagina se adapta adecuadamente a los diferentes tipos de tamaños</t>
   </si>
+  <si>
+    <t>CP-1</t>
+  </si>
+  <si>
+    <t>CP-2</t>
+  </si>
+  <si>
+    <t>CP-3</t>
+  </si>
+  <si>
+    <t>CP-4</t>
+  </si>
+  <si>
+    <t>CP-5</t>
+  </si>
+  <si>
+    <t>CP-6</t>
+  </si>
+  <si>
+    <t>CP-7</t>
+  </si>
+  <si>
+    <t>CP-8</t>
+  </si>
+  <si>
+    <t>CP-9</t>
+  </si>
+  <si>
+    <t>CP-10</t>
+  </si>
+  <si>
+    <t>CP-11</t>
+  </si>
+  <si>
+    <t>CP-12</t>
+  </si>
+  <si>
+    <t>CP-13</t>
+  </si>
 </sst>
 </file>
 
@@ -406,9 +445,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -418,6 +454,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,8 +677,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -648,30 +687,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="7" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="1"/>
@@ -693,19 +732,19 @@
     </row>
     <row r="2" spans="1:26" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="11"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -724,8 +763,8 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>1</v>
+      <c r="A3" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>10</v>
@@ -770,8 +809,8 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>2</v>
+      <c r="A4" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>18</v>
@@ -816,8 +855,8 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>3</v>
+      <c r="A5" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>24</v>
@@ -862,8 +901,8 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>4</v>
+      <c r="A6" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>30</v>
@@ -908,8 +947,8 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>5</v>
+      <c r="A7" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>35</v>
@@ -954,8 +993,8 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>6</v>
+      <c r="A8" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>39</v>
@@ -1000,8 +1039,8 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>7</v>
+      <c r="A9" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>43</v>
@@ -1046,8 +1085,8 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>8</v>
+      <c r="A10" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>48</v>
@@ -1092,8 +1131,8 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>9</v>
+      <c r="A11" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>54</v>
@@ -1138,8 +1177,8 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>10</v>
+      <c r="A12" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>59</v>
@@ -1184,8 +1223,8 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>11</v>
+      <c r="A13" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>64</v>
@@ -1230,8 +1269,8 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>12</v>
+      <c r="A14" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>69</v>
@@ -1276,8 +1315,8 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>13</v>
+      <c r="A15" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>74</v>
@@ -28903,329 +28942,89 @@
     </row>
   </sheetData>
   <mergeCells count="430">
-    <mergeCell ref="E329:F329"/>
-    <mergeCell ref="E330:F330"/>
-    <mergeCell ref="E331:F331"/>
-    <mergeCell ref="E332:F332"/>
-    <mergeCell ref="E333:F333"/>
-    <mergeCell ref="E334:F334"/>
-    <mergeCell ref="E335:F335"/>
-    <mergeCell ref="E336:F336"/>
-    <mergeCell ref="E320:F320"/>
-    <mergeCell ref="E321:F321"/>
-    <mergeCell ref="E322:F322"/>
-    <mergeCell ref="E323:F323"/>
-    <mergeCell ref="E324:F324"/>
-    <mergeCell ref="E325:F325"/>
-    <mergeCell ref="E326:F326"/>
-    <mergeCell ref="E327:F327"/>
-    <mergeCell ref="E328:F328"/>
-    <mergeCell ref="E311:F311"/>
-    <mergeCell ref="E312:F312"/>
-    <mergeCell ref="E313:F313"/>
-    <mergeCell ref="E314:F314"/>
-    <mergeCell ref="E315:F315"/>
-    <mergeCell ref="E316:F316"/>
-    <mergeCell ref="E317:F317"/>
-    <mergeCell ref="E318:F318"/>
-    <mergeCell ref="E319:F319"/>
-    <mergeCell ref="E302:F302"/>
-    <mergeCell ref="E303:F303"/>
-    <mergeCell ref="E304:F304"/>
-    <mergeCell ref="E305:F305"/>
-    <mergeCell ref="E306:F306"/>
-    <mergeCell ref="E307:F307"/>
-    <mergeCell ref="E308:F308"/>
-    <mergeCell ref="E309:F309"/>
-    <mergeCell ref="E310:F310"/>
-    <mergeCell ref="E293:F293"/>
-    <mergeCell ref="E294:F294"/>
-    <mergeCell ref="E295:F295"/>
-    <mergeCell ref="E296:F296"/>
-    <mergeCell ref="E297:F297"/>
-    <mergeCell ref="E298:F298"/>
-    <mergeCell ref="E299:F299"/>
-    <mergeCell ref="E300:F300"/>
-    <mergeCell ref="E301:F301"/>
-    <mergeCell ref="E284:F284"/>
-    <mergeCell ref="E285:F285"/>
-    <mergeCell ref="E286:F286"/>
-    <mergeCell ref="E287:F287"/>
-    <mergeCell ref="E288:F288"/>
-    <mergeCell ref="E289:F289"/>
-    <mergeCell ref="E290:F290"/>
-    <mergeCell ref="E291:F291"/>
-    <mergeCell ref="E292:F292"/>
-    <mergeCell ref="E275:F275"/>
-    <mergeCell ref="E276:F276"/>
-    <mergeCell ref="E277:F277"/>
-    <mergeCell ref="E278:F278"/>
-    <mergeCell ref="E279:F279"/>
-    <mergeCell ref="E280:F280"/>
-    <mergeCell ref="E281:F281"/>
-    <mergeCell ref="E282:F282"/>
-    <mergeCell ref="E283:F283"/>
-    <mergeCell ref="E266:F266"/>
-    <mergeCell ref="E267:F267"/>
-    <mergeCell ref="E268:F268"/>
-    <mergeCell ref="E269:F269"/>
-    <mergeCell ref="E270:F270"/>
-    <mergeCell ref="E271:F271"/>
-    <mergeCell ref="E272:F272"/>
-    <mergeCell ref="E273:F273"/>
-    <mergeCell ref="E274:F274"/>
-    <mergeCell ref="E257:F257"/>
-    <mergeCell ref="E258:F258"/>
-    <mergeCell ref="E259:F259"/>
-    <mergeCell ref="E260:F260"/>
-    <mergeCell ref="E261:F261"/>
-    <mergeCell ref="E262:F262"/>
-    <mergeCell ref="E263:F263"/>
-    <mergeCell ref="E264:F264"/>
-    <mergeCell ref="E265:F265"/>
-    <mergeCell ref="E248:F248"/>
-    <mergeCell ref="E249:F249"/>
-    <mergeCell ref="E250:F250"/>
-    <mergeCell ref="E251:F251"/>
-    <mergeCell ref="E252:F252"/>
-    <mergeCell ref="E253:F253"/>
-    <mergeCell ref="E254:F254"/>
-    <mergeCell ref="E255:F255"/>
-    <mergeCell ref="E256:F256"/>
-    <mergeCell ref="E239:F239"/>
-    <mergeCell ref="E240:F240"/>
-    <mergeCell ref="E241:F241"/>
-    <mergeCell ref="E242:F242"/>
-    <mergeCell ref="E243:F243"/>
-    <mergeCell ref="E244:F244"/>
-    <mergeCell ref="E245:F245"/>
-    <mergeCell ref="E246:F246"/>
-    <mergeCell ref="E247:F247"/>
-    <mergeCell ref="E230:F230"/>
-    <mergeCell ref="E231:F231"/>
-    <mergeCell ref="E232:F232"/>
-    <mergeCell ref="E233:F233"/>
-    <mergeCell ref="E234:F234"/>
-    <mergeCell ref="E235:F235"/>
-    <mergeCell ref="E236:F236"/>
-    <mergeCell ref="E237:F237"/>
-    <mergeCell ref="E238:F238"/>
-    <mergeCell ref="E221:F221"/>
-    <mergeCell ref="E222:F222"/>
-    <mergeCell ref="E223:F223"/>
-    <mergeCell ref="E224:F224"/>
-    <mergeCell ref="E225:F225"/>
-    <mergeCell ref="E226:F226"/>
-    <mergeCell ref="E227:F227"/>
-    <mergeCell ref="E228:F228"/>
-    <mergeCell ref="E229:F229"/>
-    <mergeCell ref="E212:F212"/>
-    <mergeCell ref="E213:F213"/>
-    <mergeCell ref="E214:F214"/>
-    <mergeCell ref="E215:F215"/>
-    <mergeCell ref="E216:F216"/>
-    <mergeCell ref="E217:F217"/>
-    <mergeCell ref="E218:F218"/>
-    <mergeCell ref="E219:F219"/>
-    <mergeCell ref="E220:F220"/>
-    <mergeCell ref="E203:F203"/>
-    <mergeCell ref="E204:F204"/>
-    <mergeCell ref="E205:F205"/>
-    <mergeCell ref="E206:F206"/>
-    <mergeCell ref="E207:F207"/>
-    <mergeCell ref="E208:F208"/>
-    <mergeCell ref="E209:F209"/>
-    <mergeCell ref="E210:F210"/>
-    <mergeCell ref="E211:F211"/>
-    <mergeCell ref="E194:F194"/>
-    <mergeCell ref="E195:F195"/>
-    <mergeCell ref="E196:F196"/>
-    <mergeCell ref="E197:F197"/>
-    <mergeCell ref="E198:F198"/>
-    <mergeCell ref="E199:F199"/>
-    <mergeCell ref="E200:F200"/>
-    <mergeCell ref="E201:F201"/>
-    <mergeCell ref="E202:F202"/>
-    <mergeCell ref="E185:F185"/>
-    <mergeCell ref="E186:F186"/>
-    <mergeCell ref="E187:F187"/>
-    <mergeCell ref="E188:F188"/>
-    <mergeCell ref="E189:F189"/>
-    <mergeCell ref="E190:F190"/>
-    <mergeCell ref="E191:F191"/>
-    <mergeCell ref="E192:F192"/>
-    <mergeCell ref="E193:F193"/>
-    <mergeCell ref="E176:F176"/>
-    <mergeCell ref="E177:F177"/>
-    <mergeCell ref="E178:F178"/>
-    <mergeCell ref="E179:F179"/>
-    <mergeCell ref="E180:F180"/>
-    <mergeCell ref="E181:F181"/>
-    <mergeCell ref="E182:F182"/>
-    <mergeCell ref="E183:F183"/>
-    <mergeCell ref="E184:F184"/>
-    <mergeCell ref="E167:F167"/>
-    <mergeCell ref="E168:F168"/>
-    <mergeCell ref="E169:F169"/>
-    <mergeCell ref="E170:F170"/>
-    <mergeCell ref="E171:F171"/>
-    <mergeCell ref="E172:F172"/>
-    <mergeCell ref="E173:F173"/>
-    <mergeCell ref="E174:F174"/>
-    <mergeCell ref="E175:F175"/>
-    <mergeCell ref="E158:F158"/>
-    <mergeCell ref="E159:F159"/>
-    <mergeCell ref="E160:F160"/>
-    <mergeCell ref="E161:F161"/>
-    <mergeCell ref="E162:F162"/>
-    <mergeCell ref="E163:F163"/>
-    <mergeCell ref="E164:F164"/>
-    <mergeCell ref="E165:F165"/>
-    <mergeCell ref="E166:F166"/>
-    <mergeCell ref="E149:F149"/>
-    <mergeCell ref="E150:F150"/>
-    <mergeCell ref="E151:F151"/>
-    <mergeCell ref="E152:F152"/>
-    <mergeCell ref="E153:F153"/>
-    <mergeCell ref="E154:F154"/>
-    <mergeCell ref="E155:F155"/>
-    <mergeCell ref="E156:F156"/>
-    <mergeCell ref="E157:F157"/>
-    <mergeCell ref="E140:F140"/>
-    <mergeCell ref="E141:F141"/>
-    <mergeCell ref="E142:F142"/>
-    <mergeCell ref="E143:F143"/>
-    <mergeCell ref="E144:F144"/>
-    <mergeCell ref="E145:F145"/>
-    <mergeCell ref="E146:F146"/>
-    <mergeCell ref="E147:F147"/>
-    <mergeCell ref="E148:F148"/>
-    <mergeCell ref="E131:F131"/>
-    <mergeCell ref="E132:F132"/>
-    <mergeCell ref="E133:F133"/>
-    <mergeCell ref="E134:F134"/>
-    <mergeCell ref="E135:F135"/>
-    <mergeCell ref="E136:F136"/>
-    <mergeCell ref="E137:F137"/>
-    <mergeCell ref="E138:F138"/>
-    <mergeCell ref="E139:F139"/>
-    <mergeCell ref="E122:F122"/>
-    <mergeCell ref="E123:F123"/>
-    <mergeCell ref="E124:F124"/>
-    <mergeCell ref="E125:F125"/>
-    <mergeCell ref="E126:F126"/>
-    <mergeCell ref="E127:F127"/>
-    <mergeCell ref="E128:F128"/>
-    <mergeCell ref="E129:F129"/>
-    <mergeCell ref="E130:F130"/>
-    <mergeCell ref="E113:F113"/>
-    <mergeCell ref="E114:F114"/>
-    <mergeCell ref="E115:F115"/>
-    <mergeCell ref="E116:F116"/>
-    <mergeCell ref="E117:F117"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="E119:F119"/>
-    <mergeCell ref="E120:F120"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="E104:F104"/>
-    <mergeCell ref="E105:F105"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="E107:F107"/>
-    <mergeCell ref="E108:F108"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="E95:F95"/>
-    <mergeCell ref="E96:F96"/>
-    <mergeCell ref="E97:F97"/>
-    <mergeCell ref="E98:F98"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="E100:F100"/>
-    <mergeCell ref="E101:F101"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="E103:F103"/>
-    <mergeCell ref="E86:F86"/>
-    <mergeCell ref="E87:F87"/>
-    <mergeCell ref="E88:F88"/>
-    <mergeCell ref="E89:F89"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="E91:F91"/>
-    <mergeCell ref="E92:F92"/>
-    <mergeCell ref="E93:F93"/>
-    <mergeCell ref="E94:F94"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="E80:F80"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="E82:F82"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="E84:F84"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E386:F386"/>
+    <mergeCell ref="E387:F387"/>
+    <mergeCell ref="E388:F388"/>
+    <mergeCell ref="E389:F389"/>
+    <mergeCell ref="E390:F390"/>
+    <mergeCell ref="E391:F391"/>
+    <mergeCell ref="E392:F392"/>
+    <mergeCell ref="E393:F393"/>
+    <mergeCell ref="E394:F394"/>
+    <mergeCell ref="E395:F395"/>
+    <mergeCell ref="E396:F396"/>
+    <mergeCell ref="E397:F397"/>
+    <mergeCell ref="E398:F398"/>
+    <mergeCell ref="E399:F399"/>
+    <mergeCell ref="E400:F400"/>
+    <mergeCell ref="E401:F401"/>
+    <mergeCell ref="E402:F402"/>
+    <mergeCell ref="E403:F403"/>
+    <mergeCell ref="E404:F404"/>
+    <mergeCell ref="E405:F405"/>
+    <mergeCell ref="E406:F406"/>
+    <mergeCell ref="E407:F407"/>
+    <mergeCell ref="E408:F408"/>
+    <mergeCell ref="E409:F409"/>
+    <mergeCell ref="E410:F410"/>
+    <mergeCell ref="E411:F411"/>
+    <mergeCell ref="E412:F412"/>
+    <mergeCell ref="E413:F413"/>
+    <mergeCell ref="E421:F421"/>
+    <mergeCell ref="E422:F422"/>
+    <mergeCell ref="E423:F423"/>
+    <mergeCell ref="E414:F414"/>
+    <mergeCell ref="E415:F415"/>
+    <mergeCell ref="E416:F416"/>
+    <mergeCell ref="E417:F417"/>
+    <mergeCell ref="E418:F418"/>
+    <mergeCell ref="E419:F419"/>
+    <mergeCell ref="E420:F420"/>
+    <mergeCell ref="E337:F337"/>
+    <mergeCell ref="E338:F338"/>
+    <mergeCell ref="E339:F339"/>
+    <mergeCell ref="E340:F340"/>
+    <mergeCell ref="E341:F341"/>
+    <mergeCell ref="E342:F342"/>
+    <mergeCell ref="E343:F343"/>
+    <mergeCell ref="E344:F344"/>
+    <mergeCell ref="E345:F345"/>
+    <mergeCell ref="E346:F346"/>
+    <mergeCell ref="E347:F347"/>
+    <mergeCell ref="E348:F348"/>
+    <mergeCell ref="E349:F349"/>
+    <mergeCell ref="E350:F350"/>
+    <mergeCell ref="E351:F351"/>
+    <mergeCell ref="E352:F352"/>
+    <mergeCell ref="E353:F353"/>
+    <mergeCell ref="E354:F354"/>
+    <mergeCell ref="E355:F355"/>
+    <mergeCell ref="E356:F356"/>
+    <mergeCell ref="E357:F357"/>
+    <mergeCell ref="E358:F358"/>
+    <mergeCell ref="E359:F359"/>
+    <mergeCell ref="E360:F360"/>
+    <mergeCell ref="E361:F361"/>
+    <mergeCell ref="E362:F362"/>
+    <mergeCell ref="E363:F363"/>
+    <mergeCell ref="E364:F364"/>
+    <mergeCell ref="E365:F365"/>
+    <mergeCell ref="E366:F366"/>
+    <mergeCell ref="E367:F367"/>
+    <mergeCell ref="E368:F368"/>
+    <mergeCell ref="E369:F369"/>
+    <mergeCell ref="E370:F370"/>
+    <mergeCell ref="E371:F371"/>
+    <mergeCell ref="E372:F372"/>
+    <mergeCell ref="E373:F373"/>
+    <mergeCell ref="E374:F374"/>
+    <mergeCell ref="E375:F375"/>
+    <mergeCell ref="E376:F376"/>
+    <mergeCell ref="E377:F377"/>
+    <mergeCell ref="E378:F378"/>
+    <mergeCell ref="E379:F379"/>
+    <mergeCell ref="E380:F380"/>
+    <mergeCell ref="E381:F381"/>
     <mergeCell ref="E382:F382"/>
     <mergeCell ref="E383:F383"/>
     <mergeCell ref="E384:F384"/>
@@ -29250,90 +29049,331 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E373:F373"/>
-    <mergeCell ref="E374:F374"/>
-    <mergeCell ref="E375:F375"/>
-    <mergeCell ref="E376:F376"/>
-    <mergeCell ref="E377:F377"/>
-    <mergeCell ref="E378:F378"/>
-    <mergeCell ref="E379:F379"/>
-    <mergeCell ref="E380:F380"/>
-    <mergeCell ref="E381:F381"/>
-    <mergeCell ref="E364:F364"/>
-    <mergeCell ref="E365:F365"/>
-    <mergeCell ref="E366:F366"/>
-    <mergeCell ref="E367:F367"/>
-    <mergeCell ref="E368:F368"/>
-    <mergeCell ref="E369:F369"/>
-    <mergeCell ref="E370:F370"/>
-    <mergeCell ref="E371:F371"/>
-    <mergeCell ref="E372:F372"/>
-    <mergeCell ref="E355:F355"/>
-    <mergeCell ref="E356:F356"/>
-    <mergeCell ref="E357:F357"/>
-    <mergeCell ref="E358:F358"/>
-    <mergeCell ref="E359:F359"/>
-    <mergeCell ref="E360:F360"/>
-    <mergeCell ref="E361:F361"/>
-    <mergeCell ref="E362:F362"/>
-    <mergeCell ref="E363:F363"/>
-    <mergeCell ref="E346:F346"/>
-    <mergeCell ref="E347:F347"/>
-    <mergeCell ref="E348:F348"/>
-    <mergeCell ref="E349:F349"/>
-    <mergeCell ref="E350:F350"/>
-    <mergeCell ref="E351:F351"/>
-    <mergeCell ref="E352:F352"/>
-    <mergeCell ref="E353:F353"/>
-    <mergeCell ref="E354:F354"/>
-    <mergeCell ref="E337:F337"/>
-    <mergeCell ref="E338:F338"/>
-    <mergeCell ref="E339:F339"/>
-    <mergeCell ref="E340:F340"/>
-    <mergeCell ref="E341:F341"/>
-    <mergeCell ref="E342:F342"/>
-    <mergeCell ref="E343:F343"/>
-    <mergeCell ref="E344:F344"/>
-    <mergeCell ref="E345:F345"/>
-    <mergeCell ref="E413:F413"/>
-    <mergeCell ref="E421:F421"/>
-    <mergeCell ref="E422:F422"/>
-    <mergeCell ref="E423:F423"/>
-    <mergeCell ref="E414:F414"/>
-    <mergeCell ref="E415:F415"/>
-    <mergeCell ref="E416:F416"/>
-    <mergeCell ref="E417:F417"/>
-    <mergeCell ref="E418:F418"/>
-    <mergeCell ref="E419:F419"/>
-    <mergeCell ref="E420:F420"/>
-    <mergeCell ref="E404:F404"/>
-    <mergeCell ref="E405:F405"/>
-    <mergeCell ref="E406:F406"/>
-    <mergeCell ref="E407:F407"/>
-    <mergeCell ref="E408:F408"/>
-    <mergeCell ref="E409:F409"/>
-    <mergeCell ref="E410:F410"/>
-    <mergeCell ref="E411:F411"/>
-    <mergeCell ref="E412:F412"/>
-    <mergeCell ref="E395:F395"/>
-    <mergeCell ref="E396:F396"/>
-    <mergeCell ref="E397:F397"/>
-    <mergeCell ref="E398:F398"/>
-    <mergeCell ref="E399:F399"/>
-    <mergeCell ref="E400:F400"/>
-    <mergeCell ref="E401:F401"/>
-    <mergeCell ref="E402:F402"/>
-    <mergeCell ref="E403:F403"/>
-    <mergeCell ref="E386:F386"/>
-    <mergeCell ref="E387:F387"/>
-    <mergeCell ref="E388:F388"/>
-    <mergeCell ref="E389:F389"/>
-    <mergeCell ref="E390:F390"/>
-    <mergeCell ref="E391:F391"/>
-    <mergeCell ref="E392:F392"/>
-    <mergeCell ref="E393:F393"/>
-    <mergeCell ref="E394:F394"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="E82:F82"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="E88:F88"/>
+    <mergeCell ref="E89:F89"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="E91:F91"/>
+    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="E93:F93"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="E95:F95"/>
+    <mergeCell ref="E96:F96"/>
+    <mergeCell ref="E97:F97"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="E101:F101"/>
+    <mergeCell ref="E102:F102"/>
+    <mergeCell ref="E103:F103"/>
+    <mergeCell ref="E104:F104"/>
+    <mergeCell ref="E105:F105"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="E107:F107"/>
+    <mergeCell ref="E108:F108"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="E113:F113"/>
+    <mergeCell ref="E114:F114"/>
+    <mergeCell ref="E115:F115"/>
+    <mergeCell ref="E116:F116"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="E119:F119"/>
+    <mergeCell ref="E120:F120"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="E123:F123"/>
+    <mergeCell ref="E124:F124"/>
+    <mergeCell ref="E125:F125"/>
+    <mergeCell ref="E126:F126"/>
+    <mergeCell ref="E127:F127"/>
+    <mergeCell ref="E128:F128"/>
+    <mergeCell ref="E129:F129"/>
+    <mergeCell ref="E130:F130"/>
+    <mergeCell ref="E131:F131"/>
+    <mergeCell ref="E132:F132"/>
+    <mergeCell ref="E133:F133"/>
+    <mergeCell ref="E134:F134"/>
+    <mergeCell ref="E135:F135"/>
+    <mergeCell ref="E136:F136"/>
+    <mergeCell ref="E137:F137"/>
+    <mergeCell ref="E138:F138"/>
+    <mergeCell ref="E139:F139"/>
+    <mergeCell ref="E140:F140"/>
+    <mergeCell ref="E141:F141"/>
+    <mergeCell ref="E142:F142"/>
+    <mergeCell ref="E143:F143"/>
+    <mergeCell ref="E144:F144"/>
+    <mergeCell ref="E145:F145"/>
+    <mergeCell ref="E146:F146"/>
+    <mergeCell ref="E147:F147"/>
+    <mergeCell ref="E148:F148"/>
+    <mergeCell ref="E149:F149"/>
+    <mergeCell ref="E150:F150"/>
+    <mergeCell ref="E151:F151"/>
+    <mergeCell ref="E152:F152"/>
+    <mergeCell ref="E153:F153"/>
+    <mergeCell ref="E154:F154"/>
+    <mergeCell ref="E155:F155"/>
+    <mergeCell ref="E156:F156"/>
+    <mergeCell ref="E157:F157"/>
+    <mergeCell ref="E158:F158"/>
+    <mergeCell ref="E159:F159"/>
+    <mergeCell ref="E160:F160"/>
+    <mergeCell ref="E161:F161"/>
+    <mergeCell ref="E162:F162"/>
+    <mergeCell ref="E163:F163"/>
+    <mergeCell ref="E164:F164"/>
+    <mergeCell ref="E165:F165"/>
+    <mergeCell ref="E166:F166"/>
+    <mergeCell ref="E167:F167"/>
+    <mergeCell ref="E168:F168"/>
+    <mergeCell ref="E169:F169"/>
+    <mergeCell ref="E170:F170"/>
+    <mergeCell ref="E171:F171"/>
+    <mergeCell ref="E172:F172"/>
+    <mergeCell ref="E173:F173"/>
+    <mergeCell ref="E174:F174"/>
+    <mergeCell ref="E175:F175"/>
+    <mergeCell ref="E176:F176"/>
+    <mergeCell ref="E177:F177"/>
+    <mergeCell ref="E178:F178"/>
+    <mergeCell ref="E179:F179"/>
+    <mergeCell ref="E180:F180"/>
+    <mergeCell ref="E181:F181"/>
+    <mergeCell ref="E182:F182"/>
+    <mergeCell ref="E183:F183"/>
+    <mergeCell ref="E184:F184"/>
+    <mergeCell ref="E185:F185"/>
+    <mergeCell ref="E186:F186"/>
+    <mergeCell ref="E187:F187"/>
+    <mergeCell ref="E188:F188"/>
+    <mergeCell ref="E189:F189"/>
+    <mergeCell ref="E190:F190"/>
+    <mergeCell ref="E191:F191"/>
+    <mergeCell ref="E192:F192"/>
+    <mergeCell ref="E193:F193"/>
+    <mergeCell ref="E194:F194"/>
+    <mergeCell ref="E195:F195"/>
+    <mergeCell ref="E196:F196"/>
+    <mergeCell ref="E197:F197"/>
+    <mergeCell ref="E198:F198"/>
+    <mergeCell ref="E199:F199"/>
+    <mergeCell ref="E200:F200"/>
+    <mergeCell ref="E201:F201"/>
+    <mergeCell ref="E202:F202"/>
+    <mergeCell ref="E203:F203"/>
+    <mergeCell ref="E204:F204"/>
+    <mergeCell ref="E205:F205"/>
+    <mergeCell ref="E206:F206"/>
+    <mergeCell ref="E207:F207"/>
+    <mergeCell ref="E208:F208"/>
+    <mergeCell ref="E209:F209"/>
+    <mergeCell ref="E210:F210"/>
+    <mergeCell ref="E211:F211"/>
+    <mergeCell ref="E212:F212"/>
+    <mergeCell ref="E213:F213"/>
+    <mergeCell ref="E214:F214"/>
+    <mergeCell ref="E215:F215"/>
+    <mergeCell ref="E216:F216"/>
+    <mergeCell ref="E217:F217"/>
+    <mergeCell ref="E218:F218"/>
+    <mergeCell ref="E219:F219"/>
+    <mergeCell ref="E220:F220"/>
+    <mergeCell ref="E221:F221"/>
+    <mergeCell ref="E222:F222"/>
+    <mergeCell ref="E223:F223"/>
+    <mergeCell ref="E224:F224"/>
+    <mergeCell ref="E225:F225"/>
+    <mergeCell ref="E226:F226"/>
+    <mergeCell ref="E227:F227"/>
+    <mergeCell ref="E228:F228"/>
+    <mergeCell ref="E229:F229"/>
+    <mergeCell ref="E230:F230"/>
+    <mergeCell ref="E231:F231"/>
+    <mergeCell ref="E232:F232"/>
+    <mergeCell ref="E233:F233"/>
+    <mergeCell ref="E234:F234"/>
+    <mergeCell ref="E235:F235"/>
+    <mergeCell ref="E236:F236"/>
+    <mergeCell ref="E237:F237"/>
+    <mergeCell ref="E238:F238"/>
+    <mergeCell ref="E239:F239"/>
+    <mergeCell ref="E240:F240"/>
+    <mergeCell ref="E241:F241"/>
+    <mergeCell ref="E242:F242"/>
+    <mergeCell ref="E243:F243"/>
+    <mergeCell ref="E244:F244"/>
+    <mergeCell ref="E245:F245"/>
+    <mergeCell ref="E246:F246"/>
+    <mergeCell ref="E247:F247"/>
+    <mergeCell ref="E248:F248"/>
+    <mergeCell ref="E249:F249"/>
+    <mergeCell ref="E250:F250"/>
+    <mergeCell ref="E251:F251"/>
+    <mergeCell ref="E252:F252"/>
+    <mergeCell ref="E253:F253"/>
+    <mergeCell ref="E254:F254"/>
+    <mergeCell ref="E255:F255"/>
+    <mergeCell ref="E256:F256"/>
+    <mergeCell ref="E257:F257"/>
+    <mergeCell ref="E258:F258"/>
+    <mergeCell ref="E259:F259"/>
+    <mergeCell ref="E260:F260"/>
+    <mergeCell ref="E261:F261"/>
+    <mergeCell ref="E262:F262"/>
+    <mergeCell ref="E263:F263"/>
+    <mergeCell ref="E264:F264"/>
+    <mergeCell ref="E265:F265"/>
+    <mergeCell ref="E266:F266"/>
+    <mergeCell ref="E267:F267"/>
+    <mergeCell ref="E268:F268"/>
+    <mergeCell ref="E269:F269"/>
+    <mergeCell ref="E270:F270"/>
+    <mergeCell ref="E271:F271"/>
+    <mergeCell ref="E272:F272"/>
+    <mergeCell ref="E273:F273"/>
+    <mergeCell ref="E274:F274"/>
+    <mergeCell ref="E275:F275"/>
+    <mergeCell ref="E276:F276"/>
+    <mergeCell ref="E277:F277"/>
+    <mergeCell ref="E278:F278"/>
+    <mergeCell ref="E279:F279"/>
+    <mergeCell ref="E280:F280"/>
+    <mergeCell ref="E281:F281"/>
+    <mergeCell ref="E282:F282"/>
+    <mergeCell ref="E283:F283"/>
+    <mergeCell ref="E284:F284"/>
+    <mergeCell ref="E285:F285"/>
+    <mergeCell ref="E286:F286"/>
+    <mergeCell ref="E287:F287"/>
+    <mergeCell ref="E288:F288"/>
+    <mergeCell ref="E289:F289"/>
+    <mergeCell ref="E290:F290"/>
+    <mergeCell ref="E291:F291"/>
+    <mergeCell ref="E292:F292"/>
+    <mergeCell ref="E293:F293"/>
+    <mergeCell ref="E294:F294"/>
+    <mergeCell ref="E295:F295"/>
+    <mergeCell ref="E296:F296"/>
+    <mergeCell ref="E297:F297"/>
+    <mergeCell ref="E298:F298"/>
+    <mergeCell ref="E299:F299"/>
+    <mergeCell ref="E300:F300"/>
+    <mergeCell ref="E301:F301"/>
+    <mergeCell ref="E302:F302"/>
+    <mergeCell ref="E303:F303"/>
+    <mergeCell ref="E304:F304"/>
+    <mergeCell ref="E305:F305"/>
+    <mergeCell ref="E306:F306"/>
+    <mergeCell ref="E307:F307"/>
+    <mergeCell ref="E308:F308"/>
+    <mergeCell ref="E309:F309"/>
+    <mergeCell ref="E310:F310"/>
+    <mergeCell ref="E311:F311"/>
+    <mergeCell ref="E312:F312"/>
+    <mergeCell ref="E313:F313"/>
+    <mergeCell ref="E314:F314"/>
+    <mergeCell ref="E315:F315"/>
+    <mergeCell ref="E316:F316"/>
+    <mergeCell ref="E317:F317"/>
+    <mergeCell ref="E318:F318"/>
+    <mergeCell ref="E319:F319"/>
+    <mergeCell ref="E329:F329"/>
+    <mergeCell ref="E330:F330"/>
+    <mergeCell ref="E331:F331"/>
+    <mergeCell ref="E332:F332"/>
+    <mergeCell ref="E333:F333"/>
+    <mergeCell ref="E334:F334"/>
+    <mergeCell ref="E335:F335"/>
+    <mergeCell ref="E336:F336"/>
+    <mergeCell ref="E320:F320"/>
+    <mergeCell ref="E321:F321"/>
+    <mergeCell ref="E322:F322"/>
+    <mergeCell ref="E323:F323"/>
+    <mergeCell ref="E324:F324"/>
+    <mergeCell ref="E325:F325"/>
+    <mergeCell ref="E326:F326"/>
+    <mergeCell ref="E327:F327"/>
+    <mergeCell ref="E328:F328"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Arreglado el tipo de suites de algunos tests
</commit_message>
<xml_diff>
--- a/Testing/Template Casos de Prueba - Grupo 1.xlsx
+++ b/Testing/Template Casos de Prueba - Grupo 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workshop\TechDev\Bimestre4\grupo-01\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Proyecto final\grupo-01\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4628B3-58F3-4BFB-BA55-7BE4553F10A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D725865-1EFF-411F-8091-0FFDFB6AE118}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="172">
   <si>
     <t>Id</t>
   </si>
@@ -525,6 +525,18 @@
   <si>
     <t>1 - Seleccionar una ciudad distinta    2 - Click en Buscar   3 - Verificar que la paginacion se ha reiniciado</t>
   </si>
+  <si>
+    <t>Prueba de Aceptacion</t>
+  </si>
+  <si>
+    <t>Prueba de Regresion</t>
+  </si>
+  <si>
+    <t>Prueba de Funcional</t>
+  </si>
+  <si>
+    <t>Prueba de Integracion</t>
+  </si>
 </sst>
 </file>
 
@@ -687,6 +699,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -696,9 +711,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,40 +931,40 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="26" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="9" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="1"/>
@@ -974,19 +986,19 @@
     </row>
     <row r="2" spans="1:26" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="13"/>
+      <c r="F2" s="14"/>
       <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1629,7 +1641,7 @@
         <v>92</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>22</v>
+        <v>171</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1675,7 +1687,7 @@
         <v>92</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>22</v>
+        <v>171</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1767,7 +1779,7 @@
         <v>92</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1905,7 +1917,7 @@
         <v>92</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1951,7 +1963,7 @@
         <v>92</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>22</v>
+        <v>170</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1997,7 +2009,7 @@
         <v>92</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>22</v>
+        <v>168</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2043,7 +2055,7 @@
         <v>92</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>22</v>
+        <v>171</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2089,7 +2101,7 @@
         <v>92</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>22</v>
+        <v>169</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -2135,7 +2147,7 @@
         <v>92</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>22</v>
+        <v>171</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -2181,7 +2193,7 @@
         <v>92</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -2227,7 +2239,7 @@
         <v>92</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -29436,89 +29448,329 @@
     </row>
   </sheetData>
   <mergeCells count="430">
-    <mergeCell ref="E386:F386"/>
-    <mergeCell ref="E387:F387"/>
-    <mergeCell ref="E388:F388"/>
-    <mergeCell ref="E389:F389"/>
-    <mergeCell ref="E390:F390"/>
-    <mergeCell ref="E391:F391"/>
-    <mergeCell ref="E392:F392"/>
-    <mergeCell ref="E393:F393"/>
-    <mergeCell ref="E394:F394"/>
-    <mergeCell ref="E395:F395"/>
-    <mergeCell ref="E396:F396"/>
-    <mergeCell ref="E397:F397"/>
-    <mergeCell ref="E398:F398"/>
-    <mergeCell ref="E399:F399"/>
-    <mergeCell ref="E400:F400"/>
-    <mergeCell ref="E401:F401"/>
-    <mergeCell ref="E402:F402"/>
-    <mergeCell ref="E403:F403"/>
-    <mergeCell ref="E404:F404"/>
-    <mergeCell ref="E405:F405"/>
-    <mergeCell ref="E406:F406"/>
-    <mergeCell ref="E407:F407"/>
-    <mergeCell ref="E408:F408"/>
-    <mergeCell ref="E409:F409"/>
-    <mergeCell ref="E410:F410"/>
-    <mergeCell ref="E411:F411"/>
-    <mergeCell ref="E412:F412"/>
-    <mergeCell ref="E413:F413"/>
-    <mergeCell ref="E421:F421"/>
-    <mergeCell ref="E422:F422"/>
-    <mergeCell ref="E423:F423"/>
-    <mergeCell ref="E414:F414"/>
-    <mergeCell ref="E415:F415"/>
-    <mergeCell ref="E416:F416"/>
-    <mergeCell ref="E417:F417"/>
-    <mergeCell ref="E418:F418"/>
-    <mergeCell ref="E419:F419"/>
-    <mergeCell ref="E420:F420"/>
-    <mergeCell ref="E337:F337"/>
-    <mergeCell ref="E338:F338"/>
-    <mergeCell ref="E339:F339"/>
-    <mergeCell ref="E340:F340"/>
-    <mergeCell ref="E341:F341"/>
-    <mergeCell ref="E342:F342"/>
-    <mergeCell ref="E343:F343"/>
-    <mergeCell ref="E344:F344"/>
-    <mergeCell ref="E345:F345"/>
-    <mergeCell ref="E346:F346"/>
-    <mergeCell ref="E347:F347"/>
-    <mergeCell ref="E348:F348"/>
-    <mergeCell ref="E349:F349"/>
-    <mergeCell ref="E350:F350"/>
-    <mergeCell ref="E351:F351"/>
-    <mergeCell ref="E352:F352"/>
-    <mergeCell ref="E353:F353"/>
-    <mergeCell ref="E354:F354"/>
-    <mergeCell ref="E355:F355"/>
-    <mergeCell ref="E356:F356"/>
-    <mergeCell ref="E357:F357"/>
-    <mergeCell ref="E358:F358"/>
-    <mergeCell ref="E359:F359"/>
-    <mergeCell ref="E360:F360"/>
-    <mergeCell ref="E361:F361"/>
-    <mergeCell ref="E362:F362"/>
-    <mergeCell ref="E363:F363"/>
-    <mergeCell ref="E364:F364"/>
-    <mergeCell ref="E365:F365"/>
-    <mergeCell ref="E366:F366"/>
-    <mergeCell ref="E367:F367"/>
-    <mergeCell ref="E368:F368"/>
-    <mergeCell ref="E369:F369"/>
-    <mergeCell ref="E370:F370"/>
-    <mergeCell ref="E371:F371"/>
-    <mergeCell ref="E372:F372"/>
-    <mergeCell ref="E373:F373"/>
-    <mergeCell ref="E374:F374"/>
-    <mergeCell ref="E375:F375"/>
-    <mergeCell ref="E376:F376"/>
-    <mergeCell ref="E377:F377"/>
-    <mergeCell ref="E378:F378"/>
-    <mergeCell ref="E379:F379"/>
-    <mergeCell ref="E380:F380"/>
-    <mergeCell ref="E381:F381"/>
+    <mergeCell ref="E329:F329"/>
+    <mergeCell ref="E330:F330"/>
+    <mergeCell ref="E331:F331"/>
+    <mergeCell ref="E332:F332"/>
+    <mergeCell ref="E333:F333"/>
+    <mergeCell ref="E334:F334"/>
+    <mergeCell ref="E335:F335"/>
+    <mergeCell ref="E336:F336"/>
+    <mergeCell ref="E320:F320"/>
+    <mergeCell ref="E321:F321"/>
+    <mergeCell ref="E322:F322"/>
+    <mergeCell ref="E323:F323"/>
+    <mergeCell ref="E324:F324"/>
+    <mergeCell ref="E325:F325"/>
+    <mergeCell ref="E326:F326"/>
+    <mergeCell ref="E327:F327"/>
+    <mergeCell ref="E328:F328"/>
+    <mergeCell ref="E311:F311"/>
+    <mergeCell ref="E312:F312"/>
+    <mergeCell ref="E313:F313"/>
+    <mergeCell ref="E314:F314"/>
+    <mergeCell ref="E315:F315"/>
+    <mergeCell ref="E316:F316"/>
+    <mergeCell ref="E317:F317"/>
+    <mergeCell ref="E318:F318"/>
+    <mergeCell ref="E319:F319"/>
+    <mergeCell ref="E302:F302"/>
+    <mergeCell ref="E303:F303"/>
+    <mergeCell ref="E304:F304"/>
+    <mergeCell ref="E305:F305"/>
+    <mergeCell ref="E306:F306"/>
+    <mergeCell ref="E307:F307"/>
+    <mergeCell ref="E308:F308"/>
+    <mergeCell ref="E309:F309"/>
+    <mergeCell ref="E310:F310"/>
+    <mergeCell ref="E293:F293"/>
+    <mergeCell ref="E294:F294"/>
+    <mergeCell ref="E295:F295"/>
+    <mergeCell ref="E296:F296"/>
+    <mergeCell ref="E297:F297"/>
+    <mergeCell ref="E298:F298"/>
+    <mergeCell ref="E299:F299"/>
+    <mergeCell ref="E300:F300"/>
+    <mergeCell ref="E301:F301"/>
+    <mergeCell ref="E284:F284"/>
+    <mergeCell ref="E285:F285"/>
+    <mergeCell ref="E286:F286"/>
+    <mergeCell ref="E287:F287"/>
+    <mergeCell ref="E288:F288"/>
+    <mergeCell ref="E289:F289"/>
+    <mergeCell ref="E290:F290"/>
+    <mergeCell ref="E291:F291"/>
+    <mergeCell ref="E292:F292"/>
+    <mergeCell ref="E275:F275"/>
+    <mergeCell ref="E276:F276"/>
+    <mergeCell ref="E277:F277"/>
+    <mergeCell ref="E278:F278"/>
+    <mergeCell ref="E279:F279"/>
+    <mergeCell ref="E280:F280"/>
+    <mergeCell ref="E281:F281"/>
+    <mergeCell ref="E282:F282"/>
+    <mergeCell ref="E283:F283"/>
+    <mergeCell ref="E266:F266"/>
+    <mergeCell ref="E267:F267"/>
+    <mergeCell ref="E268:F268"/>
+    <mergeCell ref="E269:F269"/>
+    <mergeCell ref="E270:F270"/>
+    <mergeCell ref="E271:F271"/>
+    <mergeCell ref="E272:F272"/>
+    <mergeCell ref="E273:F273"/>
+    <mergeCell ref="E274:F274"/>
+    <mergeCell ref="E257:F257"/>
+    <mergeCell ref="E258:F258"/>
+    <mergeCell ref="E259:F259"/>
+    <mergeCell ref="E260:F260"/>
+    <mergeCell ref="E261:F261"/>
+    <mergeCell ref="E262:F262"/>
+    <mergeCell ref="E263:F263"/>
+    <mergeCell ref="E264:F264"/>
+    <mergeCell ref="E265:F265"/>
+    <mergeCell ref="E248:F248"/>
+    <mergeCell ref="E249:F249"/>
+    <mergeCell ref="E250:F250"/>
+    <mergeCell ref="E251:F251"/>
+    <mergeCell ref="E252:F252"/>
+    <mergeCell ref="E253:F253"/>
+    <mergeCell ref="E254:F254"/>
+    <mergeCell ref="E255:F255"/>
+    <mergeCell ref="E256:F256"/>
+    <mergeCell ref="E239:F239"/>
+    <mergeCell ref="E240:F240"/>
+    <mergeCell ref="E241:F241"/>
+    <mergeCell ref="E242:F242"/>
+    <mergeCell ref="E243:F243"/>
+    <mergeCell ref="E244:F244"/>
+    <mergeCell ref="E245:F245"/>
+    <mergeCell ref="E246:F246"/>
+    <mergeCell ref="E247:F247"/>
+    <mergeCell ref="E230:F230"/>
+    <mergeCell ref="E231:F231"/>
+    <mergeCell ref="E232:F232"/>
+    <mergeCell ref="E233:F233"/>
+    <mergeCell ref="E234:F234"/>
+    <mergeCell ref="E235:F235"/>
+    <mergeCell ref="E236:F236"/>
+    <mergeCell ref="E237:F237"/>
+    <mergeCell ref="E238:F238"/>
+    <mergeCell ref="E221:F221"/>
+    <mergeCell ref="E222:F222"/>
+    <mergeCell ref="E223:F223"/>
+    <mergeCell ref="E224:F224"/>
+    <mergeCell ref="E225:F225"/>
+    <mergeCell ref="E226:F226"/>
+    <mergeCell ref="E227:F227"/>
+    <mergeCell ref="E228:F228"/>
+    <mergeCell ref="E229:F229"/>
+    <mergeCell ref="E212:F212"/>
+    <mergeCell ref="E213:F213"/>
+    <mergeCell ref="E214:F214"/>
+    <mergeCell ref="E215:F215"/>
+    <mergeCell ref="E216:F216"/>
+    <mergeCell ref="E217:F217"/>
+    <mergeCell ref="E218:F218"/>
+    <mergeCell ref="E219:F219"/>
+    <mergeCell ref="E220:F220"/>
+    <mergeCell ref="E203:F203"/>
+    <mergeCell ref="E204:F204"/>
+    <mergeCell ref="E205:F205"/>
+    <mergeCell ref="E206:F206"/>
+    <mergeCell ref="E207:F207"/>
+    <mergeCell ref="E208:F208"/>
+    <mergeCell ref="E209:F209"/>
+    <mergeCell ref="E210:F210"/>
+    <mergeCell ref="E211:F211"/>
+    <mergeCell ref="E194:F194"/>
+    <mergeCell ref="E195:F195"/>
+    <mergeCell ref="E196:F196"/>
+    <mergeCell ref="E197:F197"/>
+    <mergeCell ref="E198:F198"/>
+    <mergeCell ref="E199:F199"/>
+    <mergeCell ref="E200:F200"/>
+    <mergeCell ref="E201:F201"/>
+    <mergeCell ref="E202:F202"/>
+    <mergeCell ref="E185:F185"/>
+    <mergeCell ref="E186:F186"/>
+    <mergeCell ref="E187:F187"/>
+    <mergeCell ref="E188:F188"/>
+    <mergeCell ref="E189:F189"/>
+    <mergeCell ref="E190:F190"/>
+    <mergeCell ref="E191:F191"/>
+    <mergeCell ref="E192:F192"/>
+    <mergeCell ref="E193:F193"/>
+    <mergeCell ref="E176:F176"/>
+    <mergeCell ref="E177:F177"/>
+    <mergeCell ref="E178:F178"/>
+    <mergeCell ref="E179:F179"/>
+    <mergeCell ref="E180:F180"/>
+    <mergeCell ref="E181:F181"/>
+    <mergeCell ref="E182:F182"/>
+    <mergeCell ref="E183:F183"/>
+    <mergeCell ref="E184:F184"/>
+    <mergeCell ref="E167:F167"/>
+    <mergeCell ref="E168:F168"/>
+    <mergeCell ref="E169:F169"/>
+    <mergeCell ref="E170:F170"/>
+    <mergeCell ref="E171:F171"/>
+    <mergeCell ref="E172:F172"/>
+    <mergeCell ref="E173:F173"/>
+    <mergeCell ref="E174:F174"/>
+    <mergeCell ref="E175:F175"/>
+    <mergeCell ref="E158:F158"/>
+    <mergeCell ref="E159:F159"/>
+    <mergeCell ref="E160:F160"/>
+    <mergeCell ref="E161:F161"/>
+    <mergeCell ref="E162:F162"/>
+    <mergeCell ref="E163:F163"/>
+    <mergeCell ref="E164:F164"/>
+    <mergeCell ref="E165:F165"/>
+    <mergeCell ref="E166:F166"/>
+    <mergeCell ref="E149:F149"/>
+    <mergeCell ref="E150:F150"/>
+    <mergeCell ref="E151:F151"/>
+    <mergeCell ref="E152:F152"/>
+    <mergeCell ref="E153:F153"/>
+    <mergeCell ref="E154:F154"/>
+    <mergeCell ref="E155:F155"/>
+    <mergeCell ref="E156:F156"/>
+    <mergeCell ref="E157:F157"/>
+    <mergeCell ref="E140:F140"/>
+    <mergeCell ref="E141:F141"/>
+    <mergeCell ref="E142:F142"/>
+    <mergeCell ref="E143:F143"/>
+    <mergeCell ref="E144:F144"/>
+    <mergeCell ref="E145:F145"/>
+    <mergeCell ref="E146:F146"/>
+    <mergeCell ref="E147:F147"/>
+    <mergeCell ref="E148:F148"/>
+    <mergeCell ref="E131:F131"/>
+    <mergeCell ref="E132:F132"/>
+    <mergeCell ref="E133:F133"/>
+    <mergeCell ref="E134:F134"/>
+    <mergeCell ref="E135:F135"/>
+    <mergeCell ref="E136:F136"/>
+    <mergeCell ref="E137:F137"/>
+    <mergeCell ref="E138:F138"/>
+    <mergeCell ref="E139:F139"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="E123:F123"/>
+    <mergeCell ref="E124:F124"/>
+    <mergeCell ref="E125:F125"/>
+    <mergeCell ref="E126:F126"/>
+    <mergeCell ref="E127:F127"/>
+    <mergeCell ref="E128:F128"/>
+    <mergeCell ref="E129:F129"/>
+    <mergeCell ref="E130:F130"/>
+    <mergeCell ref="E113:F113"/>
+    <mergeCell ref="E114:F114"/>
+    <mergeCell ref="E115:F115"/>
+    <mergeCell ref="E116:F116"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="E119:F119"/>
+    <mergeCell ref="E120:F120"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="E104:F104"/>
+    <mergeCell ref="E105:F105"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="E107:F107"/>
+    <mergeCell ref="E108:F108"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="E95:F95"/>
+    <mergeCell ref="E96:F96"/>
+    <mergeCell ref="E97:F97"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="E101:F101"/>
+    <mergeCell ref="E102:F102"/>
+    <mergeCell ref="E103:F103"/>
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="E88:F88"/>
+    <mergeCell ref="E89:F89"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="E91:F91"/>
+    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="E93:F93"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="E82:F82"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
     <mergeCell ref="E382:F382"/>
     <mergeCell ref="E383:F383"/>
     <mergeCell ref="E384:F384"/>
@@ -29543,329 +29795,89 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="E80:F80"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="E82:F82"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="E84:F84"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="E86:F86"/>
-    <mergeCell ref="E87:F87"/>
-    <mergeCell ref="E88:F88"/>
-    <mergeCell ref="E89:F89"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="E91:F91"/>
-    <mergeCell ref="E92:F92"/>
-    <mergeCell ref="E93:F93"/>
-    <mergeCell ref="E94:F94"/>
-    <mergeCell ref="E95:F95"/>
-    <mergeCell ref="E96:F96"/>
-    <mergeCell ref="E97:F97"/>
-    <mergeCell ref="E98:F98"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="E100:F100"/>
-    <mergeCell ref="E101:F101"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="E103:F103"/>
-    <mergeCell ref="E104:F104"/>
-    <mergeCell ref="E105:F105"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="E107:F107"/>
-    <mergeCell ref="E108:F108"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="E113:F113"/>
-    <mergeCell ref="E114:F114"/>
-    <mergeCell ref="E115:F115"/>
-    <mergeCell ref="E116:F116"/>
-    <mergeCell ref="E117:F117"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="E119:F119"/>
-    <mergeCell ref="E120:F120"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="E122:F122"/>
-    <mergeCell ref="E123:F123"/>
-    <mergeCell ref="E124:F124"/>
-    <mergeCell ref="E125:F125"/>
-    <mergeCell ref="E126:F126"/>
-    <mergeCell ref="E127:F127"/>
-    <mergeCell ref="E128:F128"/>
-    <mergeCell ref="E129:F129"/>
-    <mergeCell ref="E130:F130"/>
-    <mergeCell ref="E131:F131"/>
-    <mergeCell ref="E132:F132"/>
-    <mergeCell ref="E133:F133"/>
-    <mergeCell ref="E134:F134"/>
-    <mergeCell ref="E135:F135"/>
-    <mergeCell ref="E136:F136"/>
-    <mergeCell ref="E137:F137"/>
-    <mergeCell ref="E138:F138"/>
-    <mergeCell ref="E139:F139"/>
-    <mergeCell ref="E140:F140"/>
-    <mergeCell ref="E141:F141"/>
-    <mergeCell ref="E142:F142"/>
-    <mergeCell ref="E143:F143"/>
-    <mergeCell ref="E144:F144"/>
-    <mergeCell ref="E145:F145"/>
-    <mergeCell ref="E146:F146"/>
-    <mergeCell ref="E147:F147"/>
-    <mergeCell ref="E148:F148"/>
-    <mergeCell ref="E149:F149"/>
-    <mergeCell ref="E150:F150"/>
-    <mergeCell ref="E151:F151"/>
-    <mergeCell ref="E152:F152"/>
-    <mergeCell ref="E153:F153"/>
-    <mergeCell ref="E154:F154"/>
-    <mergeCell ref="E155:F155"/>
-    <mergeCell ref="E156:F156"/>
-    <mergeCell ref="E157:F157"/>
-    <mergeCell ref="E158:F158"/>
-    <mergeCell ref="E159:F159"/>
-    <mergeCell ref="E160:F160"/>
-    <mergeCell ref="E161:F161"/>
-    <mergeCell ref="E162:F162"/>
-    <mergeCell ref="E163:F163"/>
-    <mergeCell ref="E164:F164"/>
-    <mergeCell ref="E165:F165"/>
-    <mergeCell ref="E166:F166"/>
-    <mergeCell ref="E167:F167"/>
-    <mergeCell ref="E168:F168"/>
-    <mergeCell ref="E169:F169"/>
-    <mergeCell ref="E170:F170"/>
-    <mergeCell ref="E171:F171"/>
-    <mergeCell ref="E172:F172"/>
-    <mergeCell ref="E173:F173"/>
-    <mergeCell ref="E174:F174"/>
-    <mergeCell ref="E175:F175"/>
-    <mergeCell ref="E176:F176"/>
-    <mergeCell ref="E177:F177"/>
-    <mergeCell ref="E178:F178"/>
-    <mergeCell ref="E179:F179"/>
-    <mergeCell ref="E180:F180"/>
-    <mergeCell ref="E181:F181"/>
-    <mergeCell ref="E182:F182"/>
-    <mergeCell ref="E183:F183"/>
-    <mergeCell ref="E184:F184"/>
-    <mergeCell ref="E185:F185"/>
-    <mergeCell ref="E186:F186"/>
-    <mergeCell ref="E187:F187"/>
-    <mergeCell ref="E188:F188"/>
-    <mergeCell ref="E189:F189"/>
-    <mergeCell ref="E190:F190"/>
-    <mergeCell ref="E191:F191"/>
-    <mergeCell ref="E192:F192"/>
-    <mergeCell ref="E193:F193"/>
-    <mergeCell ref="E194:F194"/>
-    <mergeCell ref="E195:F195"/>
-    <mergeCell ref="E196:F196"/>
-    <mergeCell ref="E197:F197"/>
-    <mergeCell ref="E198:F198"/>
-    <mergeCell ref="E199:F199"/>
-    <mergeCell ref="E200:F200"/>
-    <mergeCell ref="E201:F201"/>
-    <mergeCell ref="E202:F202"/>
-    <mergeCell ref="E203:F203"/>
-    <mergeCell ref="E204:F204"/>
-    <mergeCell ref="E205:F205"/>
-    <mergeCell ref="E206:F206"/>
-    <mergeCell ref="E207:F207"/>
-    <mergeCell ref="E208:F208"/>
-    <mergeCell ref="E209:F209"/>
-    <mergeCell ref="E210:F210"/>
-    <mergeCell ref="E211:F211"/>
-    <mergeCell ref="E212:F212"/>
-    <mergeCell ref="E213:F213"/>
-    <mergeCell ref="E214:F214"/>
-    <mergeCell ref="E215:F215"/>
-    <mergeCell ref="E216:F216"/>
-    <mergeCell ref="E217:F217"/>
-    <mergeCell ref="E218:F218"/>
-    <mergeCell ref="E219:F219"/>
-    <mergeCell ref="E220:F220"/>
-    <mergeCell ref="E221:F221"/>
-    <mergeCell ref="E222:F222"/>
-    <mergeCell ref="E223:F223"/>
-    <mergeCell ref="E224:F224"/>
-    <mergeCell ref="E225:F225"/>
-    <mergeCell ref="E226:F226"/>
-    <mergeCell ref="E227:F227"/>
-    <mergeCell ref="E228:F228"/>
-    <mergeCell ref="E229:F229"/>
-    <mergeCell ref="E230:F230"/>
-    <mergeCell ref="E231:F231"/>
-    <mergeCell ref="E232:F232"/>
-    <mergeCell ref="E233:F233"/>
-    <mergeCell ref="E234:F234"/>
-    <mergeCell ref="E235:F235"/>
-    <mergeCell ref="E236:F236"/>
-    <mergeCell ref="E237:F237"/>
-    <mergeCell ref="E238:F238"/>
-    <mergeCell ref="E239:F239"/>
-    <mergeCell ref="E240:F240"/>
-    <mergeCell ref="E241:F241"/>
-    <mergeCell ref="E242:F242"/>
-    <mergeCell ref="E243:F243"/>
-    <mergeCell ref="E244:F244"/>
-    <mergeCell ref="E245:F245"/>
-    <mergeCell ref="E246:F246"/>
-    <mergeCell ref="E247:F247"/>
-    <mergeCell ref="E248:F248"/>
-    <mergeCell ref="E249:F249"/>
-    <mergeCell ref="E250:F250"/>
-    <mergeCell ref="E251:F251"/>
-    <mergeCell ref="E252:F252"/>
-    <mergeCell ref="E253:F253"/>
-    <mergeCell ref="E254:F254"/>
-    <mergeCell ref="E255:F255"/>
-    <mergeCell ref="E256:F256"/>
-    <mergeCell ref="E257:F257"/>
-    <mergeCell ref="E258:F258"/>
-    <mergeCell ref="E259:F259"/>
-    <mergeCell ref="E260:F260"/>
-    <mergeCell ref="E261:F261"/>
-    <mergeCell ref="E262:F262"/>
-    <mergeCell ref="E263:F263"/>
-    <mergeCell ref="E264:F264"/>
-    <mergeCell ref="E265:F265"/>
-    <mergeCell ref="E266:F266"/>
-    <mergeCell ref="E267:F267"/>
-    <mergeCell ref="E268:F268"/>
-    <mergeCell ref="E269:F269"/>
-    <mergeCell ref="E270:F270"/>
-    <mergeCell ref="E271:F271"/>
-    <mergeCell ref="E272:F272"/>
-    <mergeCell ref="E273:F273"/>
-    <mergeCell ref="E274:F274"/>
-    <mergeCell ref="E275:F275"/>
-    <mergeCell ref="E276:F276"/>
-    <mergeCell ref="E277:F277"/>
-    <mergeCell ref="E278:F278"/>
-    <mergeCell ref="E279:F279"/>
-    <mergeCell ref="E280:F280"/>
-    <mergeCell ref="E281:F281"/>
-    <mergeCell ref="E282:F282"/>
-    <mergeCell ref="E283:F283"/>
-    <mergeCell ref="E284:F284"/>
-    <mergeCell ref="E285:F285"/>
-    <mergeCell ref="E286:F286"/>
-    <mergeCell ref="E287:F287"/>
-    <mergeCell ref="E288:F288"/>
-    <mergeCell ref="E289:F289"/>
-    <mergeCell ref="E290:F290"/>
-    <mergeCell ref="E291:F291"/>
-    <mergeCell ref="E292:F292"/>
-    <mergeCell ref="E293:F293"/>
-    <mergeCell ref="E294:F294"/>
-    <mergeCell ref="E295:F295"/>
-    <mergeCell ref="E296:F296"/>
-    <mergeCell ref="E297:F297"/>
-    <mergeCell ref="E298:F298"/>
-    <mergeCell ref="E299:F299"/>
-    <mergeCell ref="E300:F300"/>
-    <mergeCell ref="E301:F301"/>
-    <mergeCell ref="E302:F302"/>
-    <mergeCell ref="E303:F303"/>
-    <mergeCell ref="E304:F304"/>
-    <mergeCell ref="E305:F305"/>
-    <mergeCell ref="E306:F306"/>
-    <mergeCell ref="E307:F307"/>
-    <mergeCell ref="E308:F308"/>
-    <mergeCell ref="E309:F309"/>
-    <mergeCell ref="E310:F310"/>
-    <mergeCell ref="E311:F311"/>
-    <mergeCell ref="E312:F312"/>
-    <mergeCell ref="E313:F313"/>
-    <mergeCell ref="E314:F314"/>
-    <mergeCell ref="E315:F315"/>
-    <mergeCell ref="E316:F316"/>
-    <mergeCell ref="E317:F317"/>
-    <mergeCell ref="E318:F318"/>
-    <mergeCell ref="E319:F319"/>
-    <mergeCell ref="E329:F329"/>
-    <mergeCell ref="E330:F330"/>
-    <mergeCell ref="E331:F331"/>
-    <mergeCell ref="E332:F332"/>
-    <mergeCell ref="E333:F333"/>
-    <mergeCell ref="E334:F334"/>
-    <mergeCell ref="E335:F335"/>
-    <mergeCell ref="E336:F336"/>
-    <mergeCell ref="E320:F320"/>
-    <mergeCell ref="E321:F321"/>
-    <mergeCell ref="E322:F322"/>
-    <mergeCell ref="E323:F323"/>
-    <mergeCell ref="E324:F324"/>
-    <mergeCell ref="E325:F325"/>
-    <mergeCell ref="E326:F326"/>
-    <mergeCell ref="E327:F327"/>
-    <mergeCell ref="E328:F328"/>
+    <mergeCell ref="E373:F373"/>
+    <mergeCell ref="E374:F374"/>
+    <mergeCell ref="E375:F375"/>
+    <mergeCell ref="E376:F376"/>
+    <mergeCell ref="E377:F377"/>
+    <mergeCell ref="E378:F378"/>
+    <mergeCell ref="E379:F379"/>
+    <mergeCell ref="E380:F380"/>
+    <mergeCell ref="E381:F381"/>
+    <mergeCell ref="E364:F364"/>
+    <mergeCell ref="E365:F365"/>
+    <mergeCell ref="E366:F366"/>
+    <mergeCell ref="E367:F367"/>
+    <mergeCell ref="E368:F368"/>
+    <mergeCell ref="E369:F369"/>
+    <mergeCell ref="E370:F370"/>
+    <mergeCell ref="E371:F371"/>
+    <mergeCell ref="E372:F372"/>
+    <mergeCell ref="E355:F355"/>
+    <mergeCell ref="E356:F356"/>
+    <mergeCell ref="E357:F357"/>
+    <mergeCell ref="E358:F358"/>
+    <mergeCell ref="E359:F359"/>
+    <mergeCell ref="E360:F360"/>
+    <mergeCell ref="E361:F361"/>
+    <mergeCell ref="E362:F362"/>
+    <mergeCell ref="E363:F363"/>
+    <mergeCell ref="E346:F346"/>
+    <mergeCell ref="E347:F347"/>
+    <mergeCell ref="E348:F348"/>
+    <mergeCell ref="E349:F349"/>
+    <mergeCell ref="E350:F350"/>
+    <mergeCell ref="E351:F351"/>
+    <mergeCell ref="E352:F352"/>
+    <mergeCell ref="E353:F353"/>
+    <mergeCell ref="E354:F354"/>
+    <mergeCell ref="E337:F337"/>
+    <mergeCell ref="E338:F338"/>
+    <mergeCell ref="E339:F339"/>
+    <mergeCell ref="E340:F340"/>
+    <mergeCell ref="E341:F341"/>
+    <mergeCell ref="E342:F342"/>
+    <mergeCell ref="E343:F343"/>
+    <mergeCell ref="E344:F344"/>
+    <mergeCell ref="E345:F345"/>
+    <mergeCell ref="E413:F413"/>
+    <mergeCell ref="E421:F421"/>
+    <mergeCell ref="E422:F422"/>
+    <mergeCell ref="E423:F423"/>
+    <mergeCell ref="E414:F414"/>
+    <mergeCell ref="E415:F415"/>
+    <mergeCell ref="E416:F416"/>
+    <mergeCell ref="E417:F417"/>
+    <mergeCell ref="E418:F418"/>
+    <mergeCell ref="E419:F419"/>
+    <mergeCell ref="E420:F420"/>
+    <mergeCell ref="E404:F404"/>
+    <mergeCell ref="E405:F405"/>
+    <mergeCell ref="E406:F406"/>
+    <mergeCell ref="E407:F407"/>
+    <mergeCell ref="E408:F408"/>
+    <mergeCell ref="E409:F409"/>
+    <mergeCell ref="E410:F410"/>
+    <mergeCell ref="E411:F411"/>
+    <mergeCell ref="E412:F412"/>
+    <mergeCell ref="E395:F395"/>
+    <mergeCell ref="E396:F396"/>
+    <mergeCell ref="E397:F397"/>
+    <mergeCell ref="E398:F398"/>
+    <mergeCell ref="E399:F399"/>
+    <mergeCell ref="E400:F400"/>
+    <mergeCell ref="E401:F401"/>
+    <mergeCell ref="E402:F402"/>
+    <mergeCell ref="E403:F403"/>
+    <mergeCell ref="E386:F386"/>
+    <mergeCell ref="E387:F387"/>
+    <mergeCell ref="E388:F388"/>
+    <mergeCell ref="E389:F389"/>
+    <mergeCell ref="E390:F390"/>
+    <mergeCell ref="E391:F391"/>
+    <mergeCell ref="E392:F392"/>
+    <mergeCell ref="E393:F393"/>
+    <mergeCell ref="E394:F394"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>